<commit_message>
upgrades, leave button added
</commit_message>
<xml_diff>
--- a/Zoombot/PythonTimetable.xlsx
+++ b/Zoombot/PythonTimetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyCharm\ZoomBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shvmt\Documents\GitHub\Zoom-bot\Zoombot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A220FCEF-D2EB-408A-B880-942141DF5A4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E365EDBD-21D6-4847-A6AC-7E35A04E978F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="3195" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PythonTimetable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t xml:space="preserve">TIME </t>
   </si>
@@ -40,48 +40,12 @@
     <t>FRIDAY</t>
   </si>
   <si>
-    <t>SATURDAY</t>
-  </si>
-  <si>
-    <t>ssee1</t>
-  </si>
-  <si>
-    <t>cied4</t>
-  </si>
-  <si>
-    <t>csed21</t>
-  </si>
-  <si>
-    <t>scbc5</t>
-  </si>
-  <si>
-    <t>tietsom2</t>
-  </si>
-  <si>
     <t>csed3</t>
   </si>
   <si>
-    <t>mee13</t>
-  </si>
-  <si>
-    <t>tietsom3</t>
-  </si>
-  <si>
-    <t>csed12</t>
-  </si>
-  <si>
-    <t>csed32</t>
-  </si>
-  <si>
-    <t>scbc7</t>
-  </si>
-  <si>
     <t>10:30</t>
   </si>
   <si>
-    <t>11:20</t>
-  </si>
-  <si>
     <t>12:10</t>
   </si>
   <si>
@@ -110,6 +74,54 @@
   </si>
   <si>
     <t>08:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csed3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mee13 </t>
+  </si>
+  <si>
+    <t>csed2</t>
+  </si>
+  <si>
+    <t>csed4</t>
+  </si>
+  <si>
+    <t>csed9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csed5 </t>
+  </si>
+  <si>
+    <t>mee10</t>
+  </si>
+  <si>
+    <t>csed6</t>
+  </si>
+  <si>
+    <t>eied10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eied4 </t>
+  </si>
+  <si>
+    <t>csed1</t>
+  </si>
+  <si>
+    <t>csed7</t>
+  </si>
+  <si>
+    <t>eied5</t>
+  </si>
+  <si>
+    <t>eced18</t>
+  </si>
+  <si>
+    <t>eied4</t>
+  </si>
+  <si>
+    <t>11:40</t>
   </si>
 </sst>
 </file>
@@ -953,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +976,7 @@
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -983,143 +995,161 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
       </c>
-      <c r="B2">
-        <v>8653197433</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>8653197433</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>8653197433</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>8473779133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11">
-        <v>9270854060</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
   </sheetData>

</xml_diff>